<commit_message>
añadido nombre al excel
</commit_message>
<xml_diff>
--- a/datosExcel.xls.xlsx
+++ b/datosExcel.xls.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bdb2f473880fb267/Escritorio/TPE-TIO15/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D35F5AF1-D552-4B06-8426-6683E769258B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="15120" windowHeight="9144"/>
+    <workbookView xWindow="1530" yWindow="1530" windowWidth="15120" windowHeight="9150"/>
   </bookViews>
   <sheets>
     <sheet name="datosExcel" sheetId="1" r:id="rId1"/>
@@ -20,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>integrantes del grupo 15</t>
   </si>
@@ -30,11 +24,14 @@
   <si>
     <t>fermin ondicol</t>
   </si>
+  <si>
+    <t>agustin molina</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -534,11 +531,10 @@
     <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
     <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Buena" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
     <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
@@ -555,6 +551,7 @@
     <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Título 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
@@ -861,7 +858,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -869,13 +866,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
@@ -892,6 +889,11 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
agregue mi nombre al excel
</commit_message>
<xml_diff>
--- a/datosExcel.xls.xlsx
+++ b/datosExcel.xls.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Note\Desktop\TPE TIO\TPE-TIO15\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
@@ -19,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>integrantes del grupo 15</t>
   </si>
@@ -38,12 +33,18 @@
   <si>
     <t>Nahuel Gulias</t>
   </si>
+  <si>
+    <t>Sofia Corral</t>
+  </si>
+  <si>
+    <t>Jeronimo Alsua</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -61,6 +62,28 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -84,10 +107,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -304,46 +330,59 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A1000"/>
+  <dimension ref="A1:B1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="26" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="7" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
     </row>
     <row r="21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="22" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>

</xml_diff>